<commit_message>
update change variables use
</commit_message>
<xml_diff>
--- a/EmailAssignment/AssignedEmail.xlsx
+++ b/EmailAssignment/AssignedEmail.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PHAM HAI LONG\Documents\UiPath\EmailAutomationRPA\EmailAssignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F410553-6C02-4B4C-B551-81D1D17A2BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C17B51-4602-4477-AB2A-A5F8F3501546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
     <x:workbookView xWindow="-100" yWindow="-100" windowWidth="21467" windowHeight="11443" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -106,6 +106,9 @@
     <x:t>Done</x:t>
   </x:si>
   <x:si>
+    <x:t/>
+  </x:si>
+  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
@@ -129,9 +132,6 @@
   </x:si>
   <x:si>
     <x:t>Sales</x:t>
-  </x:si>
-  <x:si>
-    <x:t/>
   </x:si>
   <x:si>
     <x:t>3</x:t>
@@ -194,9 +194,6 @@
     <x:t>Others</x:t>
   </x:si>
   <x:si>
-    <x:t>2025-10-14 23:27:07</x:t>
-  </x:si>
-  <x:si>
     <x:t>6</x:t>
   </x:si>
   <x:si>
@@ -218,9 +215,6 @@
     <x:t>Compliment</x:t>
   </x:si>
   <x:si>
-    <x:t>2025-10-14 23:27:09</x:t>
-  </x:si>
-  <x:si>
     <x:t>7</x:t>
   </x:si>
   <x:si>
@@ -239,9 +233,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2025-10-14 23:27:10</x:t>
-  </x:si>
-  <x:si>
     <x:t>8</x:t>
   </x:si>
   <x:si>
@@ -257,9 +248,6 @@
 Best regards,
 Thương Hiền.
 </x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-10-14 23:27:12</x:t>
   </x:si>
   <x:si>
     <x:t>9</x:t>
@@ -280,9 +268,6 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2025-10-14 23:27:14</x:t>
-  </x:si>
-  <x:si>
     <x:t>10</x:t>
   </x:si>
   <x:si>
@@ -362,13 +347,16 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t>2025-10-15 00:13:28</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-10-15 00:13:30</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2025-10-15 00:13:32</x:t>
+    <x:t>2025-10-15 07:43:37</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-15 07:43:39</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2025-10-15 07:43:41</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Overdue - Reported</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -726,8 +714,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:N14"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" topLeftCell="F5" zoomScale="89" zoomScaleNormal="99" workbookViewId="0">
-      <x:selection activeCell="I5" sqref="I5"/>
+    <x:sheetView tabSelected="1" topLeftCell="F13" zoomScale="89" zoomScaleNormal="99" workbookViewId="0">
+      <x:selection activeCell="J15" sqref="J15"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -829,12 +817,12 @@
         <x:v>45947.9770023148</x:v>
       </x:c>
       <x:c r="N2" s="1" t="s">
-        <x:v>14</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>15</x:v>
@@ -843,19 +831,19 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G3" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H3" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I3" s="1" t="s">
         <x:v>16</x:v>
@@ -864,7 +852,7 @@
         <x:v>45941.9770833333</x:v>
       </x:c>
       <x:c r="K3" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="L3" s="1" t="s">
         <x:v>24</x:v>
@@ -873,7 +861,7 @@
         <x:v>45947.9770717593</x:v>
       </x:c>
       <x:c r="N3" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:14" ht="144" customHeight="1" x14ac:dyDescent="0.3">
@@ -905,7 +893,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J4" s="3">
-        <x:v>45944.9771180556</x:v>
+        <x:v>45943.9771180556</x:v>
       </x:c>
       <x:c r="K4" s="1" t="s">
         <x:v>23</x:v>
@@ -917,7 +905,7 @@
         <x:v>45947.9770949074</x:v>
       </x:c>
       <x:c r="N4" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:14" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -949,7 +937,7 @@
         <x:v>42</x:v>
       </x:c>
       <x:c r="J5" s="3">
-        <x:v>45941.9771412037</x:v>
+        <x:v>45943.9771412037</x:v>
       </x:c>
       <x:c r="K5" s="1" t="s">
         <x:v>43</x:v>
@@ -961,7 +949,7 @@
         <x:v>45947.9771180556</x:v>
       </x:c>
       <x:c r="N5" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="6" spans="1:14" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -992,8 +980,8 @@
       <x:c r="I6" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J6" s="1" t="s">
-        <x:v>49</x:v>
+      <x:c r="J6" s="3">
+        <x:v>45943.9771643519</x:v>
       </x:c>
       <x:c r="K6" s="1" t="s">
         <x:v>23</x:v>
@@ -1005,12 +993,12 @@
         <x:v>45947.9771412037</x:v>
       </x:c>
       <x:c r="N6" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:14" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A7" s="1" t="s">
-        <x:v>50</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B7" s="1" t="s">
         <x:v>15</x:v>
@@ -1019,25 +1007,25 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D7" s="1" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="E7" s="1" t="s">
         <x:v>51</x:v>
       </x:c>
-      <x:c r="E7" s="1" t="s">
+      <x:c r="F7" s="2" t="s">
         <x:v>52</x:v>
-      </x:c>
-      <x:c r="F7" s="2" t="s">
-        <x:v>53</x:v>
       </x:c>
       <x:c r="G7" s="1" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="H7" s="1" t="s">
-        <x:v>54</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="I7" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J7" s="1" t="s">
-        <x:v>55</x:v>
+      <x:c r="J7" s="3">
+        <x:v>45943.9771875</x:v>
       </x:c>
       <x:c r="K7" s="1" t="s">
         <x:v>23</x:v>
@@ -1049,12 +1037,12 @@
         <x:v>45947.9771643519</x:v>
       </x:c>
       <x:c r="N7" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:14" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A8" s="1" t="s">
-        <x:v>56</x:v>
+        <x:v>54</x:v>
       </x:c>
       <x:c r="B8" s="1" t="s">
         <x:v>15</x:v>
@@ -1063,13 +1051,13 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D8" s="1" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="E8" s="1" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="F8" s="2" t="s">
         <x:v>57</x:v>
-      </x:c>
-      <x:c r="E8" s="1" t="s">
-        <x:v>58</x:v>
-      </x:c>
-      <x:c r="F8" s="2" t="s">
-        <x:v>59</x:v>
       </x:c>
       <x:c r="G8" s="1" t="s">
         <x:v>20</x:v>
@@ -1080,8 +1068,8 @@
       <x:c r="I8" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J8" s="1" t="s">
-        <x:v>60</x:v>
+      <x:c r="J8" s="3">
+        <x:v>45943.9771990741</x:v>
       </x:c>
       <x:c r="K8" s="1" t="s">
         <x:v>23</x:v>
@@ -1093,12 +1081,12 @@
         <x:v>45947.9771875</x:v>
       </x:c>
       <x:c r="N8" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>14</x:v>
       </x:c>
     </x:row>
     <x:row r="9" spans="1:14" ht="144" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A9" s="1" t="s">
-        <x:v>61</x:v>
+        <x:v>58</x:v>
       </x:c>
       <x:c r="B9" s="1" t="s">
         <x:v>15</x:v>
@@ -1107,16 +1095,16 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D9" s="1" t="s">
-        <x:v>62</x:v>
+        <x:v>59</x:v>
       </x:c>
       <x:c r="E9" s="1" t="s">
-        <x:v>63</x:v>
+        <x:v>60</x:v>
       </x:c>
       <x:c r="F9" s="2" t="s">
-        <x:v>64</x:v>
+        <x:v>61</x:v>
       </x:c>
       <x:c r="G9" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H9" s="1" t="s">
         <x:v>48</x:v>
@@ -1124,25 +1112,25 @@
       <x:c r="I9" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J9" s="1" t="s">
-        <x:v>65</x:v>
+      <x:c r="J9" s="3">
+        <x:v>45942.9772222222</x:v>
       </x:c>
       <x:c r="K9" s="1" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="L9" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="M9" s="3">
         <x:v>45947.9771990741</x:v>
       </x:c>
-      <x:c r="N9" s="1" t="s">
-        <x:v>32</x:v>
+      <x:c r="N9" s="1">
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="10" spans="1:14" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A10" s="1" t="s">
-        <x:v>66</x:v>
+        <x:v>62</x:v>
       </x:c>
       <x:c r="B10" s="1" t="s">
         <x:v>15</x:v>
@@ -1151,16 +1139,16 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D10" s="1" t="s">
-        <x:v>67</x:v>
+        <x:v>63</x:v>
       </x:c>
       <x:c r="E10" s="1" t="s">
-        <x:v>68</x:v>
+        <x:v>64</x:v>
       </x:c>
       <x:c r="F10" s="2" t="s">
-        <x:v>69</x:v>
+        <x:v>65</x:v>
       </x:c>
       <x:c r="G10" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H10" s="1" t="s">
         <x:v>48</x:v>
@@ -1168,25 +1156,25 @@
       <x:c r="I10" s="1" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="J10" s="1" t="s">
-        <x:v>70</x:v>
+      <x:c r="J10" s="3">
+        <x:v>45942.9772453704</x:v>
       </x:c>
       <x:c r="K10" s="1" t="s">
         <x:v>23</x:v>
       </x:c>
       <x:c r="L10" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="M10" s="3">
         <x:v>45947.9772222222</x:v>
       </x:c>
-      <x:c r="N10" s="1" t="s">
-        <x:v>32</x:v>
+      <x:c r="N10" s="1">
+        <x:v>1</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A11" s="1" t="s">
-        <x:v>71</x:v>
+        <x:v>66</x:v>
       </x:c>
       <x:c r="B11" s="1" t="s">
         <x:v>15</x:v>
@@ -1195,13 +1183,13 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D11" s="1" t="s">
-        <x:v>72</x:v>
+        <x:v>67</x:v>
       </x:c>
       <x:c r="E11" s="1" t="s">
-        <x:v>73</x:v>
+        <x:v>68</x:v>
       </x:c>
       <x:c r="F11" s="2" t="s">
-        <x:v>74</x:v>
+        <x:v>69</x:v>
       </x:c>
       <x:c r="G11" s="1" t="s">
         <x:v>20</x:v>
@@ -1213,7 +1201,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J11" s="1" t="s">
-        <x:v>75</x:v>
+        <x:v>70</x:v>
       </x:c>
       <x:c r="K11" s="1" t="s">
         <x:v>23</x:v>
@@ -1225,12 +1213,12 @@
         <x:v>45947.9772453704</x:v>
       </x:c>
       <x:c r="N11" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="12" spans="1:14" ht="115.2" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A12" s="1" t="s">
-        <x:v>76</x:v>
+        <x:v>71</x:v>
       </x:c>
       <x:c r="B12" s="1" t="s">
         <x:v>15</x:v>
@@ -1239,13 +1227,13 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D12" s="1" t="s">
-        <x:v>77</x:v>
+        <x:v>72</x:v>
       </x:c>
       <x:c r="E12" s="1" t="s">
-        <x:v>78</x:v>
+        <x:v>73</x:v>
       </x:c>
       <x:c r="F12" s="2" t="s">
-        <x:v>79</x:v>
+        <x:v>74</x:v>
       </x:c>
       <x:c r="G12" s="1" t="s">
         <x:v>20</x:v>
@@ -1257,7 +1245,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J12" s="1" t="s">
-        <x:v>80</x:v>
+        <x:v>75</x:v>
       </x:c>
       <x:c r="K12" s="1" t="s">
         <x:v>23</x:v>
@@ -1269,12 +1257,12 @@
         <x:v>45947.9772685185</x:v>
       </x:c>
       <x:c r="N12" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="13" spans="1:14" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A13" s="1" t="s">
-        <x:v>81</x:v>
+        <x:v>76</x:v>
       </x:c>
       <x:c r="B13" s="1" t="s">
         <x:v>15</x:v>
@@ -1283,16 +1271,16 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D13" s="1" t="s">
-        <x:v>82</x:v>
+        <x:v>77</x:v>
       </x:c>
       <x:c r="E13" s="1" t="s">
-        <x:v>83</x:v>
+        <x:v>78</x:v>
       </x:c>
       <x:c r="F13" s="2" t="s">
-        <x:v>84</x:v>
+        <x:v>79</x:v>
       </x:c>
       <x:c r="G13" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H13" s="1" t="s">
         <x:v>21</x:v>
@@ -1301,7 +1289,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J13" s="1" t="s">
-        <x:v>85</x:v>
+        <x:v>80</x:v>
       </x:c>
       <x:c r="K13" s="1" t="s">
         <x:v>23</x:v>
@@ -1313,12 +1301,12 @@
         <x:v>45947.9772916667</x:v>
       </x:c>
       <x:c r="N13" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="14" spans="1:14" ht="129.6" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A14" s="1" t="s">
-        <x:v>86</x:v>
+        <x:v>81</x:v>
       </x:c>
       <x:c r="B14" s="1" t="s">
         <x:v>15</x:v>
@@ -1327,31 +1315,31 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D14" s="1" t="s">
-        <x:v>87</x:v>
+        <x:v>82</x:v>
       </x:c>
       <x:c r="E14" s="1" t="s">
-        <x:v>88</x:v>
+        <x:v>83</x:v>
       </x:c>
       <x:c r="F14" s="2" t="s">
-        <x:v>89</x:v>
+        <x:v>84</x:v>
       </x:c>
       <x:c r="G14" s="1" t="s">
         <x:v>40</x:v>
       </x:c>
       <x:c r="H14" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I14" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="J14" s="3">
-        <x:v>45943.977337963</x:v>
+        <x:v>45942.977337963</x:v>
       </x:c>
       <x:c r="K14" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="L14" s="1" t="s">
-        <x:v>35</x:v>
+        <x:v>88</x:v>
       </x:c>
       <x:c r="M14" s="3">
         <x:v>45947.9773148148</x:v>
@@ -1376,8 +1364,8 @@
   </x:sheetPr>
   <x:dimension ref="A1:N4"/>
   <x:sheetViews>
-    <x:sheetView topLeftCell="E2" workbookViewId="0">
-      <x:selection activeCell="N2" sqref="N2"/>
+    <x:sheetView topLeftCell="E1" workbookViewId="0">
+      <x:selection activeCell="L2" sqref="L2"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1459,7 +1447,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J2" s="1" t="s">
-        <x:v>90</x:v>
+        <x:v>85</x:v>
       </x:c>
       <x:c r="K2" s="1" t="s">
         <x:v>23</x:v>
@@ -1468,15 +1456,15 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="M2" s="3">
-        <x:v>45948.0093055556</x:v>
+        <x:v>45947.3218865741</x:v>
       </x:c>
       <x:c r="N2" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:14" ht="100.8" customHeight="1" x14ac:dyDescent="0.3">
       <x:c r="A3" s="1" t="s">
-        <x:v>25</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="B3" s="1" t="s">
         <x:v>15</x:v>
@@ -1485,37 +1473,37 @@
         <x:v>16</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
-        <x:v>26</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="E3" s="1" t="s">
-        <x:v>27</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F3" s="2" t="s">
-        <x:v>28</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="G3" s="1" t="s">
-        <x:v>29</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="H3" s="1" t="s">
-        <x:v>30</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="I3" s="1" t="s">
         <x:v>16</x:v>
       </x:c>
       <x:c r="J3" s="1" t="s">
-        <x:v>91</x:v>
+        <x:v>86</x:v>
       </x:c>
       <x:c r="K3" s="1" t="s">
-        <x:v>31</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="L3" s="1" t="s">
         <x:v>35</x:v>
       </x:c>
       <x:c r="M3" s="3">
-        <x:v>45948.0093518519</x:v>
+        <x:v>45947.3219560185</x:v>
       </x:c>
       <x:c r="N3" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:14" ht="187.2" customHeight="1" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -1547,7 +1535,7 @@
         <x:v>22</x:v>
       </x:c>
       <x:c r="J4" s="1" t="s">
-        <x:v>92</x:v>
+        <x:v>87</x:v>
       </x:c>
       <x:c r="K4" s="1" t="s">
         <x:v>23</x:v>
@@ -1556,10 +1544,10 @@
         <x:v>35</x:v>
       </x:c>
       <x:c r="M4" s="3">
-        <x:v>45948.009375</x:v>
+        <x:v>45947.3219791667</x:v>
       </x:c>
       <x:c r="N4" s="1" t="s">
-        <x:v>32</x:v>
+        <x:v>25</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>